<commit_message>
Commit with edited code and graph
</commit_message>
<xml_diff>
--- a/income.xlsx
+++ b/income.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\income\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9822F6CC-2AD7-404F-92EF-9FDE0069DB9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709A0539-60F2-498B-B5F3-8ED5CE83DD5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1F726453-9597-4F46-9CDF-9A564AB1C52D}"/>
   </bookViews>
@@ -34,94 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>Q4 2013</t>
-  </si>
-  <si>
-    <t>Q1 2014</t>
-  </si>
-  <si>
-    <t>Q2 2014</t>
-  </si>
-  <si>
-    <t>Q3 2014</t>
-  </si>
-  <si>
-    <t>Q4 2014</t>
-  </si>
-  <si>
-    <t>Q1 2015</t>
-  </si>
-  <si>
-    <t>Q2 2015</t>
-  </si>
-  <si>
-    <t>Q3 2015</t>
-  </si>
-  <si>
-    <t>Q4 2015</t>
-  </si>
-  <si>
-    <t>Q1 2016</t>
-  </si>
-  <si>
-    <t>Q2 2016</t>
-  </si>
-  <si>
-    <t>Q3 2016</t>
-  </si>
-  <si>
-    <t>Q4 2016</t>
-  </si>
-  <si>
-    <t>Q1 2017</t>
-  </si>
-  <si>
-    <t>Q2 2017</t>
-  </si>
-  <si>
-    <t>Q3 2017</t>
-  </si>
-  <si>
-    <t>Q4 2017</t>
-  </si>
-  <si>
-    <t>Q1 2018</t>
-  </si>
-  <si>
-    <t>Q2 2018</t>
-  </si>
-  <si>
-    <t>Q3 2018</t>
-  </si>
-  <si>
-    <t>Q4 2018</t>
-  </si>
-  <si>
-    <t>Q1 2019</t>
-  </si>
-  <si>
-    <t>Q2 2019</t>
-  </si>
-  <si>
-    <t>Q3 2019</t>
-  </si>
-  <si>
-    <t>Q4 2019</t>
-  </si>
-  <si>
-    <t>Q1 2020</t>
-  </si>
-  <si>
-    <t>Q2 2020</t>
-  </si>
-  <si>
-    <t>Q3 2020</t>
-  </si>
-  <si>
-    <t>Q4 2020</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Quarter</t>
   </si>
@@ -170,9 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,246 +404,249 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2" s="2">
+        <v>41609</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3" s="2">
+        <v>41699</v>
       </c>
       <c r="B3">
         <v>71.7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="A4" s="2">
+        <v>41791</v>
       </c>
       <c r="B4">
         <v>84.892799999999994</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5" s="2">
+        <v>41883</v>
       </c>
       <c r="B5">
         <v>86.335977600000007</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6" s="2">
+        <v>41974</v>
       </c>
       <c r="B6">
         <v>96.523623000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>5</v>
+      <c r="A7" s="2">
+        <v>42064</v>
       </c>
       <c r="B7">
         <v>71.813575499999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
+      <c r="A8" s="2">
+        <v>42156</v>
       </c>
       <c r="B8">
         <v>82.729239000000007</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="A9" s="2">
+        <v>42248</v>
       </c>
       <c r="B9">
         <v>81.4883004</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>8</v>
+      <c r="A10" s="2">
+        <v>42339</v>
       </c>
       <c r="B10">
         <v>97.378518900000003</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>9</v>
+      <c r="A11" s="2">
+        <v>42430</v>
       </c>
       <c r="B11">
         <v>69.917776599999996</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>10</v>
+      <c r="A12" s="2">
+        <v>42522</v>
       </c>
       <c r="B12">
         <v>78.517663099999993</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>11</v>
+      <c r="A13" s="2">
+        <v>42614</v>
       </c>
       <c r="B13">
         <v>78.360627800000003</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>12</v>
+      <c r="A14" s="2">
+        <v>42705</v>
       </c>
       <c r="B14">
         <v>91.917016399999994</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>13</v>
+      <c r="A15" s="2">
+        <v>42795</v>
       </c>
       <c r="B15">
         <v>70.132683499999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>14</v>
+      <c r="A16" s="2">
+        <v>42887</v>
       </c>
       <c r="B16">
         <v>78.057676799999996</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>15</v>
+      <c r="A17" s="2">
+        <v>42979</v>
       </c>
       <c r="B17">
         <v>77.667388399999993</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>16</v>
+      <c r="A18" s="2">
+        <v>43070</v>
       </c>
       <c r="B18">
         <v>91.802853099999993</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>17</v>
+      <c r="A19" s="2">
+        <v>43160</v>
       </c>
       <c r="B19">
         <v>70.779999700000005</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>18</v>
+      <c r="A20" s="2">
+        <v>43252</v>
       </c>
       <c r="B20">
         <v>78.141119700000004</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>19</v>
+      <c r="A21" s="2">
+        <v>43344</v>
       </c>
       <c r="B21">
         <v>77.5941318</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>20</v>
+      <c r="A22" s="2">
+        <v>43435</v>
       </c>
       <c r="B22">
         <v>90.940322499999994</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>21</v>
+      <c r="A23" s="2">
+        <v>43525</v>
       </c>
       <c r="B23">
         <v>69.206523799999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>22</v>
+      <c r="A24" s="2">
+        <v>43617</v>
       </c>
       <c r="B24">
         <v>78.549400199999994</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>23</v>
+      <c r="A25" s="2">
+        <v>43709</v>
       </c>
       <c r="B25">
         <v>79.413443599999994</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>24</v>
+      <c r="A26" s="2">
+        <v>43800</v>
       </c>
       <c r="B26">
         <v>93.072555899999998</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>25</v>
+      <c r="A27" s="2">
+        <v>43891</v>
       </c>
       <c r="B27">
         <v>69.804416900000007</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>26</v>
+      <c r="A28" s="2">
+        <v>43983</v>
       </c>
       <c r="B28">
         <v>72.317375900000002</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>27</v>
+      <c r="A29" s="2">
+        <v>44075</v>
       </c>
       <c r="B29">
         <v>75.210070999999999</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>28</v>
+      <c r="A30" s="2">
+        <v>44166</v>
       </c>
       <c r="B30">
         <v>91.455446300000006</v>

</xml_diff>